<commit_message>
Have Jakobs implementation of Petri net here with questions and notes
</commit_message>
<xml_diff>
--- a/skema.xlsx
+++ b/skema.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barth\Documents\studie\Master thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barth\Documents\studie\master thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680397AA-0D1C-4269-8006-691034DF61D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52685F4-CAC4-4D12-AF9A-842E37F766C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="14">
   <si>
     <t>mandag</t>
   </si>
@@ -472,7 +472,7 @@
   <dimension ref="B5:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,7 +955,9 @@
       <c r="D24" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="3"/>
+      <c r="E24" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -970,11 +972,11 @@
       </c>
       <c r="N24">
         <f>SUM(N25:N31)</f>
-        <v>15.5</v>
+        <v>23.5</v>
       </c>
       <c r="O24">
         <f>SUM(O25:O31)+P24</f>
-        <v>15.5</v>
+        <v>23.5</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
@@ -987,7 +989,9 @@
       <c r="D25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="3"/>
+      <c r="E25" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -1022,7 +1026,9 @@
       <c r="D26" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="3"/>
+      <c r="E26" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -1057,7 +1063,9 @@
       <c r="D27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="3"/>
+      <c r="E27" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -1075,11 +1083,11 @@
       </c>
       <c r="N27">
         <f>COUNTIF(E24:E38, "*andet*")-COUNTIF(E24:E38,"*andet/2*")*0.5-COUNTIF(E24:E38,"*andet/4")*0.75</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O27">
         <f>SUM(L27:N27)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
@@ -1092,7 +1100,9 @@
       <c r="D28" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="3"/>
+      <c r="E28" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
@@ -1127,7 +1137,9 @@
       <c r="D29" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="3"/>
+      <c r="E29" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -1162,7 +1174,9 @@
       <c r="D30" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="3"/>
+      <c r="E30" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F30" s="4"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -1197,7 +1211,9 @@
       <c r="D31" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="3"/>
+      <c r="E31" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -1246,11 +1262,11 @@
       </c>
       <c r="N32">
         <f>SUM(N25:N31)/5</f>
-        <v>3.1</v>
+        <v>4.7</v>
       </c>
       <c r="O32">
         <f>SUM(O25:O31)/5</f>
-        <v>3.1</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Made example of how to access arc weights
</commit_message>
<xml_diff>
--- a/skema.xlsx
+++ b/skema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barth\Documents\studie\master thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75051ED-B92B-46BF-887D-F126625C5C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C873D446-F7C9-46A9-9515-8C5B9B71BA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="14">
   <si>
     <t>mandag</t>
   </si>
@@ -493,7 +493,7 @@
   <dimension ref="B5:O56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1450,9 +1450,15 @@
       <c r="D42" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
+      <c r="E42" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
       <c r="L42">
@@ -1465,11 +1471,11 @@
       </c>
       <c r="N42">
         <f>SUM(N43:N49)</f>
-        <v>14.5</v>
+        <v>40</v>
       </c>
       <c r="O42">
         <f>SUM(O43:O49)+P42</f>
-        <v>14.5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
@@ -1482,9 +1488,15 @@
       <c r="D43" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
+      <c r="E43" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="K43" t="s">
@@ -1517,9 +1529,15 @@
       <c r="D44" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
+      <c r="E44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
       <c r="K44" t="s">
@@ -1552,9 +1570,15 @@
       <c r="D45" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
+      <c r="E45" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
       <c r="K45" t="s">
@@ -1570,11 +1594,11 @@
       </c>
       <c r="N45">
         <f>COUNTIF(E42:E56, "*andet*")-COUNTIF(E42:E56,"*andet/2*")*0.5-COUNTIF(E42:E56,"*andet/4")*0.75</f>
-        <v>0</v>
+        <v>8.25</v>
       </c>
       <c r="O45">
         <f>SUM(L45:N45)</f>
-        <v>0</v>
+        <v>8.25</v>
       </c>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
@@ -1587,9 +1611,15 @@
       <c r="D46" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
+      <c r="E46" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
       <c r="K46" t="s">
@@ -1605,11 +1635,11 @@
       </c>
       <c r="N46">
         <f>COUNTIF(F42:F56, "*andet*")-COUNTIF(F42:F56,"*andet/2*")*0.5-COUNTIF(F42:F56,"*andet/4")*0.75</f>
-        <v>0</v>
+        <v>8.25</v>
       </c>
       <c r="O46">
         <f>SUM(L46:N46)</f>
-        <v>0</v>
+        <v>8.25</v>
       </c>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
@@ -1622,9 +1652,15 @@
       <c r="D47" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
+      <c r="E47" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
       <c r="K47" t="s">
@@ -1640,11 +1676,11 @@
       </c>
       <c r="N47">
         <f>COUNTIF(G42:G56, "*andet*")-COUNTIF(G42:G56,"*andet/2*")*0.5-COUNTIF(G42:G56,"*andet/4")*0.75</f>
-        <v>0</v>
+        <v>7.25</v>
       </c>
       <c r="O47">
         <f t="shared" ref="O47" si="5">SUM(L47:N47)</f>
-        <v>0</v>
+        <v>7.25</v>
       </c>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
@@ -1657,9 +1693,15 @@
       <c r="D48" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E48" s="3"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="3"/>
+      <c r="E48" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
       <c r="K48" t="s">
@@ -1692,9 +1734,15 @@
       <c r="D49" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
+      <c r="E49" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
       <c r="K49" t="s">
@@ -1710,11 +1758,11 @@
       </c>
       <c r="N49">
         <f>COUNTIF(I42:I56, "*andet*")-COUNTIF(I42:I56,"*andet/2*")*0.5-COUNTIF(I42:I56,"*andet/4")*0.75</f>
-        <v>0</v>
+        <v>1.75</v>
       </c>
       <c r="O49">
         <f>SUM(L49:N49)</f>
-        <v>0</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
@@ -1727,8 +1775,12 @@
       <c r="D50" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
+      <c r="E50" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
@@ -1745,11 +1797,11 @@
       </c>
       <c r="N50">
         <f>SUM(N43:N49)/5</f>
-        <v>2.9</v>
+        <v>8</v>
       </c>
       <c r="O50">
         <f>SUM(O43:O49)/5</f>
-        <v>2.9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
@@ -1798,7 +1850,9 @@
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
+      <c r="I54" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" s="2">
@@ -1810,7 +1864,9 @@
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
+      <c r="I55" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B56" s="2">
@@ -1822,7 +1878,9 @@
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
+      <c r="I56" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C6:I20">

</xml_diff>